<commit_message>
updated variable name for toggle project
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/ToggleData - Copy.xlsx
+++ b/ToggleData - Copy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="EntityorAccount" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -37,88 +37,9 @@
     <t>Record_Type</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Fax</t>
-  </si>
-  <si>
-    <t>Parent_Institution</t>
-  </si>
-  <si>
-    <t>WebSite</t>
-  </si>
-  <si>
-    <t>Employees</t>
-  </si>
-  <si>
-    <t>Bank_Name</t>
-  </si>
-  <si>
-    <t>Institution Type</t>
-  </si>
-  <si>
-    <t>Fund Preferences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Industry Preferences 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Street </t>
-  </si>
-  <si>
-    <t xml:space="preserve">City </t>
-  </si>
-  <si>
-    <t xml:space="preserve">State/Province </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zip/Postal Code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shipping Street </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shipping City </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shipping State/Province </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shipping Zip/Postal Code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shipping Country </t>
-  </si>
-  <si>
-    <t>Modules</t>
-  </si>
-  <si>
     <t>Institution</t>
   </si>
   <si>
-    <t>Pre Condition</t>
-  </si>
-  <si>
-    <t>N 86</t>
-  </si>
-  <si>
-    <t>Noida</t>
-  </si>
-  <si>
-    <t>UP</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
     <t>Fund_Name</t>
   </si>
   <si>
@@ -156,6 +77,12 @@
   </si>
   <si>
     <t>Alexa Sep Deal 2020</t>
+  </si>
+  <si>
+    <t>Deal_Name</t>
+  </si>
+  <si>
+    <t>Stage</t>
   </si>
 </sst>
 </file>
@@ -194,7 +121,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,12 +140,6 @@
         <bgColor rgb="FFA9D18E"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFDEEBF7"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -234,7 +155,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -243,21 +164,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -356,8 +268,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>668160</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
@@ -404,8 +316,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>672120</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
@@ -452,8 +364,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>672840</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>168120</xdr:rowOff>
     </xdr:to>
@@ -761,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK18"/>
+  <dimension ref="A1:ALP18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,204 +684,56 @@
     <col min="1" max="1" width="15.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="41" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="21" style="2" customWidth="1"/>
-    <col min="12" max="18" width="21.7109375" style="2" customWidth="1"/>
-    <col min="19" max="19" width="25.28515625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="21.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="18.28515625" style="2" customWidth="1"/>
-    <col min="22" max="23" width="13.28515625" style="2" customWidth="1"/>
-    <col min="24" max="24" width="19" style="2" customWidth="1"/>
-    <col min="25" max="1025" width="9.140625" style="2" customWidth="1"/>
+    <col min="4" max="1004" width="9.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2"/>
-      <c r="X2" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X3" s="9"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X4" s="9"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X5" s="9"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="L6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O6" s="2">
-        <v>210310</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="V6" s="2">
-        <v>3636366336</v>
-      </c>
-      <c r="W6" s="2">
-        <v>554477331</v>
-      </c>
-      <c r="X6" s="9"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="X10" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="X11" s="9"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="X12" s="9"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="X13" s="9"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="L14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O14" s="2">
-        <v>210310</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="V14" s="2">
-        <v>3636366336</v>
-      </c>
-      <c r="W14" s="2">
-        <v>554477331</v>
-      </c>
-      <c r="X14" s="9"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
+      <c r="B18" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="X2:X6"/>
-    <mergeCell ref="X10:X14"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
@@ -978,10 +742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK12"/>
+  <dimension ref="A1:AMK11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,48 +762,48 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>38</v>
+      <c r="A2" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>39</v>
+      <c r="A3" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4"/>
@@ -1047,21 +811,13 @@
       <c r="C4"/>
       <c r="D4"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="B11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1071,10 +827,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,23 +840,26 @@
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="8" t="s">
+      <c r="B1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>41</v>
+      <c r="D1" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added precondition script for Toggle
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/ToggleData - Copy.xlsx
+++ b/ToggleData - Copy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EntityorAccount" sheetId="5" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Stage</t>
+  </si>
+  <si>
+    <t>Deal Received</t>
   </si>
 </sst>
 </file>
@@ -675,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALP18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -829,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,6 +841,7 @@
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -861,6 +865,9 @@
       <c r="B2" t="s">
         <v>16</v>
       </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Copy of Toggle Excel sheet
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/ToggleData - Copy.xlsx
+++ b/ToggleData - Copy.xlsx
@@ -9,12 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="EntityorAccount" sheetId="5" r:id="rId1"/>
     <sheet name="Fund" sheetId="6" r:id="rId2"/>
     <sheet name="Deal" sheetId="11" r:id="rId3"/>
+    <sheet name="CustomSDG" sheetId="12" r:id="rId4"/>
+    <sheet name="DealRequestTracker" sheetId="14" r:id="rId5"/>
+    <sheet name="MarketingEvent" sheetId="13" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId7"/>
+    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -86,13 +91,163 @@
   </si>
   <si>
     <t>Deal Received</t>
+  </si>
+  <si>
+    <t>SDG_Name</t>
+  </si>
+  <si>
+    <t>SDG_Tag</t>
+  </si>
+  <si>
+    <t>sObjectName</t>
+  </si>
+  <si>
+    <t>TOGGLESDG1</t>
+  </si>
+  <si>
+    <t>Custom SDG</t>
+  </si>
+  <si>
+    <t>navpeII__Pipeline__c</t>
+  </si>
+  <si>
+    <t>OPENQA1</t>
+  </si>
+  <si>
+    <t>CLOSEDQA1</t>
+  </si>
+  <si>
+    <t>Request_Tracker_ID</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>Date_Requested</t>
+  </si>
+  <si>
+    <t>Finance Related</t>
+  </si>
+  <si>
+    <t>12/22/2020</t>
+  </si>
+  <si>
+    <t>12/7/2020</t>
+  </si>
+  <si>
+    <t>IT Related</t>
+  </si>
+  <si>
+    <t>Third Party Event</t>
+  </si>
+  <si>
+    <t>Alexa Event 1</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Organizer</t>
+  </si>
+  <si>
+    <t>2/10/2020</t>
+  </si>
+  <si>
+    <t>TOGGLEME1</t>
+  </si>
+  <si>
+    <t>Marketing_Event_Name</t>
+  </si>
+  <si>
+    <t>TabNAME&lt;BREAK&gt;ITEM&lt;BREAK&gt;RELATEDTAB&lt;BREAK&gt;1,2&lt;BREAK&gt;</t>
+  </si>
+  <si>
+    <t>Onject</t>
+  </si>
+  <si>
+    <t>TabNAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thirtd party </t>
+  </si>
+  <si>
+    <t>a,b ,c d</t>
+  </si>
+  <si>
+    <t>TabName</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>RelatedTab</t>
+  </si>
+  <si>
+    <t>ToggleButton</t>
+  </si>
+  <si>
+    <t>Entities</t>
+  </si>
+  <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>TBC1</t>
+  </si>
+  <si>
+    <t>TBC2</t>
+  </si>
+  <si>
+    <t>TBC3</t>
+  </si>
+  <si>
+    <t>Deals</t>
+  </si>
+  <si>
+    <t>Marketing Events</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Q&amp;A</t>
+  </si>
+  <si>
+    <t>Column_Name</t>
+  </si>
+  <si>
+    <t>Fund Investments&lt;break&gt;Co-Investments</t>
+  </si>
+  <si>
+    <t>Open Questions&lt;break&gt;Closed</t>
+  </si>
+  <si>
+    <t>Third Party Event&lt;break&gt;Our Events</t>
+  </si>
+  <si>
+    <t>Legal Entity&lt;column&gt;Fund&lt;column&gt;Commitment Amount(M)&lt;column&gt;Commitment Date&lt;break&gt;Legal Entity&lt;column&gt;Asset&lt;column&gt;Commitment Amount(M)&lt;column&gt;Commitment Date</t>
+  </si>
+  <si>
+    <t>Request Tracker ID&lt;column&gt;Date Requested&lt;column&gt;Request&lt;column&gt;Status&lt;break&gt;Request Tracker ID&lt;column&gt;Date Requested&lt;column&gt;Request</t>
+  </si>
+  <si>
+    <t>Name&lt;column&gt;Title&lt;column&gt;Email&lt;break&gt;Staff Name&lt;column&gt;Title&lt;column&gt;Mobile Phone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -123,8 +278,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +304,12 @@
         <bgColor rgb="FFA9D18E"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -158,7 +325,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,6 +341,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink 2" xfId="1"/>
@@ -679,7 +849,7 @@
   <dimension ref="A1:ALP18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +875,7 @@
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -748,7 +918,7 @@
   <dimension ref="A1:AMK11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,4 +1042,333 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="108.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="127.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>